<commit_message>
intento fallido de arreglar vbp
</commit_message>
<xml_diff>
--- a/analisis/resultados/argentina/renta_comparacion_autores.xlsx
+++ b/analisis/resultados/argentina/renta_comparacion_autores.xlsx
@@ -4388,7 +4388,7 @@
         </is>
       </c>
       <c r="E176">
-        <v>-30.93416599986339</v>
+        <v>-30.93447024799347</v>
       </c>
     </row>
     <row r="177">
@@ -4411,7 +4411,7 @@
         </is>
       </c>
       <c r="E177">
-        <v>70.13177669489221</v>
+        <v>70.13063190173146</v>
       </c>
     </row>
     <row r="178">
@@ -4434,7 +4434,7 @@
         </is>
       </c>
       <c r="E178">
-        <v>106.0268385703013</v>
+        <v>104.9350680740262</v>
       </c>
     </row>
     <row r="179">
@@ -4457,7 +4457,7 @@
         </is>
       </c>
       <c r="E179">
-        <v>282.6997534533968</v>
+        <v>282.7077624933602</v>
       </c>
     </row>
     <row r="180">
@@ -4480,7 +4480,7 @@
         </is>
       </c>
       <c r="E180">
-        <v>-61.9424631918772</v>
+        <v>-61.94102716304131</v>
       </c>
     </row>
     <row r="181">
@@ -4503,7 +4503,7 @@
         </is>
       </c>
       <c r="E181">
-        <v>-186.2774730564882</v>
+        <v>-186.2591787303295</v>
       </c>
     </row>
     <row r="182">
@@ -4526,7 +4526,7 @@
         </is>
       </c>
       <c r="E182">
-        <v>-76.39121877173776</v>
+        <v>-78.34435110789292</v>
       </c>
     </row>
     <row r="183">
@@ -4549,7 +4549,7 @@
         </is>
       </c>
       <c r="E183">
-        <v>91.7491861434649</v>
+        <v>91.73485762614818</v>
       </c>
     </row>
     <row r="184">
@@ -4572,7 +4572,7 @@
         </is>
       </c>
       <c r="E184">
-        <v>236.704816181236</v>
+        <v>236.7844053683192</v>
       </c>
     </row>
     <row r="185">
@@ -4595,7 +4595,7 @@
         </is>
       </c>
       <c r="E185">
-        <v>265.0485818749373</v>
+        <v>265.0308929108967</v>
       </c>
     </row>
     <row r="186">
@@ -4618,7 +4618,7 @@
         </is>
       </c>
       <c r="E186">
-        <v>643.3731864120398</v>
+        <v>643.385941056861</v>
       </c>
     </row>
     <row r="187">
@@ -4641,7 +4641,7 @@
         </is>
       </c>
       <c r="E187">
-        <v>1610.853329373624</v>
+        <v>1610.870180503204</v>
       </c>
     </row>
     <row r="188">
@@ -4664,7 +4664,7 @@
         </is>
       </c>
       <c r="E188">
-        <v>1704.80013323767</v>
+        <v>1704.815308530421</v>
       </c>
     </row>
     <row r="189">
@@ -4687,7 +4687,7 @@
         </is>
       </c>
       <c r="E189">
-        <v>1466.83071741738</v>
+        <v>1466.856164287803</v>
       </c>
     </row>
     <row r="190">
@@ -4710,7 +4710,7 @@
         </is>
       </c>
       <c r="E190">
-        <v>1801.450833508913</v>
+        <v>1801.472644663213</v>
       </c>
     </row>
     <row r="191">
@@ -4733,7 +4733,7 @@
         </is>
       </c>
       <c r="E191">
-        <v>1787.1762318873</v>
+        <v>1787.168739195896</v>
       </c>
     </row>
     <row r="192">
@@ -4756,7 +4756,7 @@
         </is>
       </c>
       <c r="E192">
-        <v>4947.705289355234</v>
+        <v>4947.69068161478</v>
       </c>
     </row>
     <row r="193">
@@ -4779,7 +4779,7 @@
         </is>
       </c>
       <c r="E193">
-        <v>6305.321283146856</v>
+        <v>6305.362121755735</v>
       </c>
     </row>
     <row r="194">
@@ -4802,7 +4802,7 @@
         </is>
       </c>
       <c r="E194">
-        <v>6437.540761328651</v>
+        <v>6437.612137187783</v>
       </c>
     </row>
     <row r="195">
@@ -4825,7 +4825,7 @@
         </is>
       </c>
       <c r="E195">
-        <v>5761.306861343483</v>
+        <v>5761.323671830959</v>
       </c>
     </row>
     <row r="196">
@@ -4848,7 +4848,7 @@
         </is>
       </c>
       <c r="E196">
-        <v>4196.992004204276</v>
+        <v>4197.004020233644</v>
       </c>
     </row>
     <row r="197">
@@ -4871,7 +4871,7 @@
         </is>
       </c>
       <c r="E197">
-        <v>4404.781407327527</v>
+        <v>4404.803048276855</v>
       </c>
     </row>
     <row r="198">
@@ -4894,7 +4894,7 @@
         </is>
       </c>
       <c r="E198">
-        <v>3606.199145283455</v>
+        <v>3606.204688076076</v>
       </c>
     </row>
     <row r="199">
@@ -4917,7 +4917,7 @@
         </is>
       </c>
       <c r="E199">
-        <v>2546.968168203092</v>
+        <v>2546.964920951899</v>
       </c>
     </row>
     <row r="200">
@@ -4940,7 +4940,7 @@
         </is>
       </c>
       <c r="E200">
-        <v>2243.756777140258</v>
+        <v>2243.764741000658</v>
       </c>
     </row>
     <row r="201">
@@ -4963,7 +4963,7 @@
         </is>
       </c>
       <c r="E201">
-        <v>809.8220686141972</v>
+        <v>809.8180589883409</v>
       </c>
     </row>
     <row r="202">
@@ -4986,7 +4986,7 @@
         </is>
       </c>
       <c r="E202">
-        <v>3650.616537329649</v>
+        <v>3650.642101717535</v>
       </c>
     </row>
     <row r="203">
@@ -5009,7 +5009,7 @@
         </is>
       </c>
       <c r="E203">
-        <v>3626.633243641759</v>
+        <v>3626.6362723304</v>
       </c>
     </row>
     <row r="204">
@@ -5032,7 +5032,7 @@
         </is>
       </c>
       <c r="E204">
-        <v>4742.198020551375</v>
+        <v>4742.145264779835</v>
       </c>
     </row>
     <row r="205">
@@ -5055,7 +5055,7 @@
         </is>
       </c>
       <c r="E205">
-        <v>3631.216113686618</v>
+        <v>3631.224856667284</v>
       </c>
     </row>
     <row r="206">
@@ -5078,7 +5078,7 @@
         </is>
       </c>
       <c r="E206">
-        <v>2192.521169112788</v>
+        <v>2192.156119528132</v>
       </c>
     </row>
     <row r="207">
@@ -5101,7 +5101,7 @@
         </is>
       </c>
       <c r="E207">
-        <v>2039.553879271167</v>
+        <v>2038.949164093487</v>
       </c>
     </row>
     <row r="208">
@@ -5124,7 +5124,7 @@
         </is>
       </c>
       <c r="E208">
-        <v>2515.947208563899</v>
+        <v>2515.947197298002</v>
       </c>
     </row>
     <row r="209">
@@ -5147,7 +5147,7 @@
         </is>
       </c>
       <c r="E209">
-        <v>3047.868804120387</v>
+        <v>3047.868824296746</v>
       </c>
     </row>
     <row r="210">
@@ -5170,7 +5170,7 @@
         </is>
       </c>
       <c r="E210">
-        <v>2753.643396760613</v>
+        <v>2753.643386373699</v>
       </c>
     </row>
     <row r="211">
@@ -5193,7 +5193,7 @@
         </is>
       </c>
       <c r="E211">
-        <v>1614.181567306336</v>
+        <v>1614.181567687775</v>
       </c>
     </row>
     <row r="212">
@@ -5216,7 +5216,7 @@
         </is>
       </c>
       <c r="E212">
-        <v>2198.507270600949</v>
+        <v>2077.639145860988</v>
       </c>
     </row>
     <row r="213">
@@ -5239,7 +5239,7 @@
         </is>
       </c>
       <c r="E213">
-        <v>4569.419960096972</v>
+        <v>4433.171726884147</v>
       </c>
     </row>
     <row r="214">
@@ -5262,7 +5262,7 @@
         </is>
       </c>
       <c r="E214">
-        <v>3486.45529832734</v>
+        <v>3316.748111702572</v>
       </c>
     </row>
     <row r="215">
@@ -5285,7 +5285,7 @@
         </is>
       </c>
       <c r="E215">
-        <v>3417.498657431463</v>
+        <v>3440.098260076793</v>
       </c>
     </row>
     <row r="216">
@@ -5308,7 +5308,7 @@
         </is>
       </c>
       <c r="E216">
-        <v>3068.891247637955</v>
+        <v>3044.108096525371</v>
       </c>
     </row>
     <row r="217">
@@ -5331,7 +5331,7 @@
         </is>
       </c>
       <c r="E217">
-        <v>4380.02820512641</v>
+        <v>4323.037906831347</v>
       </c>
     </row>
     <row r="218">
@@ -5354,7 +5354,7 @@
         </is>
       </c>
       <c r="E218">
-        <v>7315.97570127422</v>
+        <v>7118.760904441265</v>
       </c>
     </row>
     <row r="219">
@@ -5377,7 +5377,7 @@
         </is>
       </c>
       <c r="E219">
-        <v>10603.74597765677</v>
+        <v>10357.79276158131</v>
       </c>
     </row>
     <row r="220">
@@ -5400,7 +5400,7 @@
         </is>
       </c>
       <c r="E220">
-        <v>12187.04886635174</v>
+        <v>11945.32220106251</v>
       </c>
     </row>
     <row r="221">
@@ -5423,7 +5423,7 @@
         </is>
       </c>
       <c r="E221">
-        <v>29115.65045661416</v>
+        <v>28841.23591783809</v>
       </c>
     </row>
     <row r="222">
@@ -5446,7 +5446,7 @@
         </is>
       </c>
       <c r="E222">
-        <v>15463.13957475798</v>
+        <v>15603.75819405868</v>
       </c>
     </row>
     <row r="223">
@@ -5469,7 +5469,7 @@
         </is>
       </c>
       <c r="E223">
-        <v>20800.77693465019</v>
+        <v>21085.2297379748</v>
       </c>
     </row>
     <row r="224">
@@ -5492,7 +5492,7 @@
         </is>
       </c>
       <c r="E224">
-        <v>27542.80947079045</v>
+        <v>27993.43024244759</v>
       </c>
     </row>
     <row r="225">
@@ -5515,7 +5515,7 @@
         </is>
       </c>
       <c r="E225">
-        <v>29710.79694637829</v>
+        <v>30146.1357396349</v>
       </c>
     </row>
     <row r="226">
@@ -5538,7 +5538,7 @@
         </is>
       </c>
       <c r="E226">
-        <v>24408.65337826184</v>
+        <v>24751.17534990787</v>
       </c>
     </row>
     <row r="227">
@@ -5561,7 +5561,7 @@
         </is>
       </c>
       <c r="E227">
-        <v>22172.54892691648</v>
+        <v>22461.11208471438</v>
       </c>
     </row>
     <row r="228">
@@ -5584,7 +5584,7 @@
         </is>
       </c>
       <c r="E228">
-        <v>8193.406042783405</v>
+        <v>8216.331359362774</v>
       </c>
     </row>
     <row r="229">
@@ -5607,7 +5607,7 @@
         </is>
       </c>
       <c r="E229">
-        <v>3229.456426580603</v>
+        <v>3230.964899539834</v>
       </c>
     </row>
     <row r="230">
@@ -5630,7 +5630,7 @@
         </is>
       </c>
       <c r="E230">
-        <v>5784.45354285194</v>
+        <v>5754.990786191625</v>
       </c>
     </row>
     <row r="231">
@@ -5653,7 +5653,7 @@
         </is>
       </c>
       <c r="E231">
-        <v>5446.809589277445</v>
+        <v>5489.060682059311</v>
       </c>
     </row>
     <row r="232">
@@ -7044,7 +7044,7 @@
         </is>
       </c>
       <c r="E292">
-        <v>-30.91267883662923</v>
+        <v>-30.91298308475931</v>
       </c>
     </row>
     <row r="293">
@@ -7067,7 +7067,7 @@
         </is>
       </c>
       <c r="E293">
-        <v>70.10767730897753</v>
+        <v>70.10653251581678</v>
       </c>
     </row>
     <row r="294">
@@ -7090,7 +7090,7 @@
         </is>
       </c>
       <c r="E294">
-        <v>106.0265353317594</v>
+        <v>104.9347648354843</v>
       </c>
     </row>
     <row r="295">
@@ -7113,7 +7113,7 @@
         </is>
       </c>
       <c r="E295">
-        <v>282.6814903648405</v>
+        <v>282.6894994048039</v>
       </c>
     </row>
     <row r="296">
@@ -7136,7 +7136,7 @@
         </is>
       </c>
       <c r="E296">
-        <v>-61.94153473034842</v>
+        <v>-61.94009870151253</v>
       </c>
     </row>
     <row r="297">
@@ -7159,7 +7159,7 @@
         </is>
       </c>
       <c r="E297">
-        <v>-186.2894911037026</v>
+        <v>-186.2711967775439</v>
       </c>
     </row>
     <row r="298">
@@ -7182,7 +7182,7 @@
         </is>
       </c>
       <c r="E298">
-        <v>-76.34996764292775</v>
+        <v>-78.30309997908293</v>
       </c>
     </row>
     <row r="299">
@@ -7205,7 +7205,7 @@
         </is>
       </c>
       <c r="E299">
-        <v>91.7491861434649</v>
+        <v>91.73485762614818</v>
       </c>
     </row>
     <row r="300">
@@ -7228,7 +7228,7 @@
         </is>
       </c>
       <c r="E300">
-        <v>236.704816181236</v>
+        <v>236.7844053683192</v>
       </c>
     </row>
     <row r="301">
@@ -7251,7 +7251,7 @@
         </is>
       </c>
       <c r="E301">
-        <v>265.0485822650676</v>
+        <v>265.0308933010269</v>
       </c>
     </row>
     <row r="302">
@@ -7274,7 +7274,7 @@
         </is>
       </c>
       <c r="E302">
-        <v>643.3731864120398</v>
+        <v>643.3859410568612</v>
       </c>
     </row>
     <row r="303">
@@ -7297,7 +7297,7 @@
         </is>
       </c>
       <c r="E303">
-        <v>1609.798889465748</v>
+        <v>1609.815740595328</v>
       </c>
     </row>
     <row r="304">
@@ -7320,7 +7320,7 @@
         </is>
       </c>
       <c r="E304">
-        <v>1704.386193422032</v>
+        <v>1704.401368714782</v>
       </c>
     </row>
     <row r="305">
@@ -7343,7 +7343,7 @@
         </is>
       </c>
       <c r="E305">
-        <v>1466.810847734898</v>
+        <v>1466.836294605321</v>
       </c>
     </row>
     <row r="306">
@@ -7366,7 +7366,7 @@
         </is>
       </c>
       <c r="E306">
-        <v>1801.406416129747</v>
+        <v>1801.428227284046</v>
       </c>
     </row>
     <row r="307">
@@ -7389,7 +7389,7 @@
         </is>
       </c>
       <c r="E307">
-        <v>1787.100451821298</v>
+        <v>1787.092959129895</v>
       </c>
     </row>
     <row r="308">
@@ -7412,7 +7412,7 @@
         </is>
       </c>
       <c r="E308">
-        <v>4947.70525849756</v>
+        <v>4947.690650757108</v>
       </c>
     </row>
     <row r="309">
@@ -7435,7 +7435,7 @@
         </is>
       </c>
       <c r="E309">
-        <v>6305.321283146857</v>
+        <v>6305.362121755735</v>
       </c>
     </row>
     <row r="310">
@@ -7458,7 +7458,7 @@
         </is>
       </c>
       <c r="E310">
-        <v>6437.540761328651</v>
+        <v>6437.612137187783</v>
       </c>
     </row>
     <row r="311">
@@ -7481,7 +7481,7 @@
         </is>
       </c>
       <c r="E311">
-        <v>5761.306861343484</v>
+        <v>5761.32367183096</v>
       </c>
     </row>
     <row r="312">
@@ -7504,7 +7504,7 @@
         </is>
       </c>
       <c r="E312">
-        <v>4196.992004204276</v>
+        <v>4197.004020233644</v>
       </c>
     </row>
     <row r="313">
@@ -7527,7 +7527,7 @@
         </is>
       </c>
       <c r="E313">
-        <v>4405.019994735347</v>
+        <v>4405.041635684676</v>
       </c>
     </row>
     <row r="314">
@@ -7550,7 +7550,7 @@
         </is>
       </c>
       <c r="E314">
-        <v>3614.627456851024</v>
+        <v>3614.632999643644</v>
       </c>
     </row>
     <row r="315">
@@ -7573,7 +7573,7 @@
         </is>
       </c>
       <c r="E315">
-        <v>2548.060970962016</v>
+        <v>2548.057723710823</v>
       </c>
     </row>
     <row r="316">
@@ -7596,7 +7596,7 @@
         </is>
       </c>
       <c r="E316">
-        <v>2244.032297024281</v>
+        <v>2244.040260884682</v>
       </c>
     </row>
     <row r="317">
@@ -7619,7 +7619,7 @@
         </is>
       </c>
       <c r="E317">
-        <v>807.575410151015</v>
+        <v>807.5714005251587</v>
       </c>
     </row>
     <row r="318">
@@ -7642,7 +7642,7 @@
         </is>
       </c>
       <c r="E318">
-        <v>3664.452387461585</v>
+        <v>3664.477951849472</v>
       </c>
     </row>
     <row r="319">
@@ -7665,7 +7665,7 @@
         </is>
       </c>
       <c r="E319">
-        <v>3566.325441255945</v>
+        <v>3566.328469944585</v>
       </c>
     </row>
     <row r="320">
@@ -7688,7 +7688,7 @@
         </is>
       </c>
       <c r="E320">
-        <v>4491.427041422969</v>
+        <v>4491.374285651429</v>
       </c>
     </row>
     <row r="321">
@@ -7711,7 +7711,7 @@
         </is>
       </c>
       <c r="E321">
-        <v>3274.87393027067</v>
+        <v>3274.882673251336</v>
       </c>
     </row>
     <row r="322">
@@ -7734,7 +7734,7 @@
         </is>
       </c>
       <c r="E322">
-        <v>1734.27681609961</v>
+        <v>1733.911766514953</v>
       </c>
     </row>
     <row r="323">
@@ -7757,7 +7757,7 @@
         </is>
       </c>
       <c r="E323">
-        <v>1516.230132065057</v>
+        <v>1515.625416887377</v>
       </c>
     </row>
     <row r="324">
@@ -7780,7 +7780,7 @@
         </is>
       </c>
       <c r="E324">
-        <v>1647.165002701442</v>
+        <v>1647.164991435544</v>
       </c>
     </row>
     <row r="325">
@@ -7803,7 +7803,7 @@
         </is>
       </c>
       <c r="E325">
-        <v>1575.7179748519</v>
+        <v>1575.717995028259</v>
       </c>
     </row>
     <row r="326">
@@ -7826,7 +7826,7 @@
         </is>
       </c>
       <c r="E326">
-        <v>1377.155621168449</v>
+        <v>1377.155610781535</v>
       </c>
     </row>
     <row r="327">
@@ -7849,7 +7849,7 @@
         </is>
       </c>
       <c r="E327">
-        <v>700.9477024250264</v>
+        <v>700.9477028064657</v>
       </c>
     </row>
     <row r="328">
@@ -7872,7 +7872,7 @@
         </is>
       </c>
       <c r="E328">
-        <v>1161.955467811923</v>
+        <v>1041.087343071962</v>
       </c>
     </row>
     <row r="329">
@@ -7895,7 +7895,7 @@
         </is>
       </c>
       <c r="E329">
-        <v>3892.990961861824</v>
+        <v>3756.742728648999</v>
       </c>
     </row>
     <row r="330">
@@ -7918,7 +7918,7 @@
         </is>
       </c>
       <c r="E330">
-        <v>1818.061423951416</v>
+        <v>1648.354237326649</v>
       </c>
     </row>
     <row r="331">
@@ -7941,7 +7941,7 @@
         </is>
       </c>
       <c r="E331">
-        <v>-485.0126834270936</v>
+        <v>-462.4130807817629</v>
       </c>
     </row>
     <row r="332">
@@ -7964,7 +7964,7 @@
         </is>
       </c>
       <c r="E332">
-        <v>143.5689288491948</v>
+        <v>118.7857777366114</v>
       </c>
     </row>
     <row r="333">
@@ -7987,7 +7987,7 @@
         </is>
       </c>
       <c r="E333">
-        <v>938.0670636025134</v>
+        <v>881.0767653074504</v>
       </c>
     </row>
     <row r="334">
@@ -8010,7 +8010,7 @@
         </is>
       </c>
       <c r="E334">
-        <v>3338.846171043388</v>
+        <v>3141.631374210432</v>
       </c>
     </row>
     <row r="335">
@@ -8033,7 +8033,7 @@
         </is>
       </c>
       <c r="E335">
-        <v>6134.709198605005</v>
+        <v>5888.75598252955</v>
       </c>
     </row>
     <row r="336">
@@ -8056,7 +8056,7 @@
         </is>
       </c>
       <c r="E336">
-        <v>8790.959558963921</v>
+        <v>8549.232893674682</v>
       </c>
     </row>
     <row r="337">
@@ -8079,7 +8079,7 @@
         </is>
       </c>
       <c r="E337">
-        <v>24122.67358620939</v>
+        <v>23848.25904743331</v>
       </c>
     </row>
     <row r="338">
@@ -8102,7 +8102,7 @@
         </is>
       </c>
       <c r="E338">
-        <v>10884.27206659987</v>
+        <v>11024.89068590057</v>
       </c>
     </row>
     <row r="339">
@@ -8125,7 +8125,7 @@
         </is>
       </c>
       <c r="E339">
-        <v>16912.45617530643</v>
+        <v>17196.90897863105</v>
       </c>
     </row>
     <row r="340">
@@ -8148,7 +8148,7 @@
         </is>
       </c>
       <c r="E340">
-        <v>23916.70793251693</v>
+        <v>24367.32870417406</v>
       </c>
     </row>
     <row r="341">
@@ -8171,7 +8171,7 @@
         </is>
       </c>
       <c r="E341">
-        <v>26202.62143211569</v>
+        <v>26637.96022537229</v>
       </c>
     </row>
     <row r="342">
@@ -8194,7 +8194,7 @@
         </is>
       </c>
       <c r="E342">
-        <v>22779.58311082285</v>
+        <v>23122.10508246888</v>
       </c>
     </row>
     <row r="343">
@@ -8217,7 +8217,7 @@
         </is>
       </c>
       <c r="E343">
-        <v>20449.6431906018</v>
+        <v>20738.2063483997</v>
       </c>
     </row>
     <row r="344">
@@ -8240,7 +8240,7 @@
         </is>
       </c>
       <c r="E344">
-        <v>8450.787029414139</v>
+        <v>8473.712345993508</v>
       </c>
     </row>
     <row r="345">
@@ -8263,7 +8263,7 @@
         </is>
       </c>
       <c r="E345">
-        <v>2253.2899911307</v>
+        <v>2254.798464089931</v>
       </c>
     </row>
     <row r="346">
@@ -8286,7 +8286,7 @@
         </is>
       </c>
       <c r="E346">
-        <v>4363.149122117408</v>
+        <v>4333.686365457092</v>
       </c>
     </row>
     <row r="347">
@@ -8309,7 +8309,7 @@
         </is>
       </c>
       <c r="E347">
-        <v>3928.057795102215</v>
+        <v>3970.308887884082</v>
       </c>
     </row>
     <row r="348">

</xml_diff>